<commit_message>
[MS-OXCNOTIF] fix work item 712067: Add 4+ new cases for NotificationData Structure
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="3510" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4287" uniqueCount="1374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4289" uniqueCount="1374">
   <si>
     <t>Req ID</t>
   </si>
@@ -4386,7 +4386,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -4667,21 +4667,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4706,189 +4691,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="53">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5227,6 +5049,184 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5356,34 +5356,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I584" tableType="xml" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" headerRowCellStyle="Normal" dataCellStyle="Normal" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I584" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal" connectionId="1">
   <autoFilter ref="A19:I584"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="50" dataCellStyle="Normal">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="49" dataCellStyle="Normal">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="48" dataCellStyle="Normal">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="47" dataCellStyle="Normal">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="46" dataCellStyle="Normal">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="45" dataCellStyle="Normal">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="44" dataCellStyle="Normal">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="43" dataCellStyle="Normal">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="42">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -5392,12 +5392,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="36"/>
-    <tableColumn id="2" name="Test" dataDxfId="35"/>
-    <tableColumn id="3" name="Description" dataDxfId="34"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5446,7 +5446,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5479,9 +5479,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5514,6 +5531,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5693,16 +5727,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L585"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C376" sqref="C376"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
@@ -5749,127 +5781,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5882,12 +5914,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -5900,12 +5932,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -5918,12 +5950,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -5936,60 +5968,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -6735,7 +6767,7 @@
         <v>15</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I47" s="31"/>
     </row>
@@ -6760,7 +6792,7 @@
         <v>15</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I48" s="31"/>
     </row>
@@ -6785,7 +6817,7 @@
         <v>15</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I49" s="31"/>
     </row>
@@ -7516,13 +7548,13 @@
         <v>19</v>
       </c>
       <c r="F78" s="34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G78" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H78" s="34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I78" s="32"/>
     </row>
@@ -7541,13 +7573,13 @@
         <v>19</v>
       </c>
       <c r="F79" s="34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G79" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H79" s="34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I79" s="32"/>
     </row>
@@ -7780,8 +7812,8 @@
       <c r="F88" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G88" s="34" t="s">
-        <v>6</v>
+      <c r="G88" s="29" t="s">
+        <v>15</v>
       </c>
       <c r="H88" s="34" t="s">
         <v>17</v>
@@ -8181,12 +8213,16 @@
       <c r="A104" s="22" t="s">
         <v>1069</v>
       </c>
-      <c r="B104" s="35"/>
+      <c r="B104" s="24" t="s">
+        <v>586</v>
+      </c>
       <c r="C104" s="32" t="s">
         <v>1067</v>
       </c>
       <c r="D104" s="34"/>
-      <c r="E104" s="34"/>
+      <c r="E104" s="34" t="s">
+        <v>19</v>
+      </c>
       <c r="F104" s="34" t="s">
         <v>6</v>
       </c>
@@ -12896,7 +12932,7 @@
         <v>15</v>
       </c>
       <c r="H284" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I284" s="31"/>
     </row>
@@ -13077,7 +13113,7 @@
         <v>15</v>
       </c>
       <c r="H291" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I291" s="31"/>
     </row>
@@ -20723,6 +20759,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -20730,154 +20771,149 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A583:B584 D583:I584 A20:I582">
-    <cfRule type="expression" dxfId="33" priority="79">
+    <cfRule type="expression" dxfId="52" priority="79">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="80">
+    <cfRule type="expression" dxfId="51" priority="80">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="87">
+    <cfRule type="expression" dxfId="50" priority="87">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A583:B584 D583:I584 A20:I582">
-    <cfRule type="expression" dxfId="30" priority="33">
+    <cfRule type="expression" dxfId="49" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="34">
+    <cfRule type="expression" dxfId="48" priority="34">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="35">
+    <cfRule type="expression" dxfId="47" priority="35">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F582:F584 G88 F20:F580">
-    <cfRule type="expression" dxfId="27" priority="39">
+    <cfRule type="expression" dxfId="46" priority="39">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="40">
+    <cfRule type="expression" dxfId="45" priority="40">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I582:I584">
-    <cfRule type="expression" dxfId="25" priority="30">
+    <cfRule type="expression" dxfId="44" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="31">
+    <cfRule type="expression" dxfId="43" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="32">
+    <cfRule type="expression" dxfId="42" priority="32">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I582:I584">
-    <cfRule type="expression" dxfId="22" priority="27">
+    <cfRule type="expression" dxfId="41" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="28">
+    <cfRule type="expression" dxfId="40" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="29">
+    <cfRule type="expression" dxfId="39" priority="29">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F581">
-    <cfRule type="expression" dxfId="19" priority="22">
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>NOT(VLOOKUP(F581,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="23">
+    <cfRule type="expression" dxfId="37" priority="23">
       <formula>(VLOOKUP(F581,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I581">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="35" priority="17">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I581">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C583">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C583">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C584">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C584">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 G88 F20:F511 F512:F584">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F584">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E511 E512:E584">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E584">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G87 G89:G511 G512:G584">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G584">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H582:H584 H20:H511 H512:H580">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H582:H584 H20:H580">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H581">
@@ -20887,7 +20923,7 @@
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B19:B49 B51:B69 B73:B77 B80:B87 B89:B103 B105:B120 B296:B412 B503:B511 B413:B498 B566:B585 B521:B565" numberStoredAsText="1"/>
+    <ignoredError sqref="B19:B295 B296:B412 B502:B520 B413:B501 B566:B585 B521:B565 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
[MS-OXCNOTIF] workitem 712070: Add new cases and capture code for 16 requirements related with 11 fixed TDIs and TDQs
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4289" uniqueCount="1374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="1375">
   <si>
     <t>Req ID</t>
   </si>
@@ -4381,6 +4381,9 @@
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] Implementation does support the session context cookie. (&lt;11&gt; Section 3.1.1:  The session context cookie was introduced in Exchange 2013 SP1.)</t>
+  </si>
+  <si>
+    <t>Verified by requirement: MS-OXCRPC_R1343.</t>
   </si>
 </sst>
 </file>
@@ -4667,6 +4670,21 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4690,21 +4708,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5781,127 +5784,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5914,12 +5917,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -5932,12 +5935,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -5950,12 +5953,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -5968,60 +5971,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -14736,9 +14739,11 @@
         <v>15</v>
       </c>
       <c r="H354" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I354" s="31"/>
+        <v>17</v>
+      </c>
+      <c r="I354" s="20" t="s">
+        <v>1374</v>
+      </c>
     </row>
     <row r="355" spans="1:9" ht="45">
       <c r="A355" s="29" t="s">
@@ -20759,11 +20764,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -20771,6 +20771,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A583:B584 D583:I584 A20:I582">

</xml_diff>

<commit_message>
[Common]: fix watchman error issue
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
@@ -3368,9 +3368,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In EcDoRpcExt2 Method (opnum 11)] [pcbOut] If the value in the pcbOut parameter on input is less than 0x00000008, the server SHOULD&lt;22&gt; fail with error code ecRpcFailed (0x80040115).</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -4384,6 +4381,9 @@
   </si>
   <si>
     <t>Verified by requirement: MS-OXCRPC_R1343.</t>
+  </si>
+  <si>
+    <t>[In EcDoRpcExt2 Method (opnum 11)] [pcbOut] If the value in the pcbOut parameter on input is less than 0x00000008, the server SHOULD&lt;21&gt; fail with error code ecRpcFailed (0x80040115).</t>
   </si>
 </sst>
 </file>
@@ -4670,21 +4670,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4708,6 +4693,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5773,7 +5773,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -5784,127 +5784,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5917,12 +5917,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -5935,12 +5935,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -5953,12 +5953,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -5971,60 +5971,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -6826,13 +6826,13 @@
     </row>
     <row r="50" spans="1:9" ht="30">
       <c r="A50" s="22" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B50" s="30" t="s">
         <v>578</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D50" s="34"/>
       <c r="E50" s="29" t="s">
@@ -7131,7 +7131,7 @@
         <v>17</v>
       </c>
       <c r="I61" s="20" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -7142,7 +7142,7 @@
         <v>581</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29" t="s">
@@ -7167,7 +7167,7 @@
         <v>581</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29" t="s">
@@ -7183,7 +7183,7 @@
         <v>17</v>
       </c>
       <c r="I63" s="20" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="45">
@@ -7194,7 +7194,7 @@
         <v>581</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -7219,7 +7219,7 @@
         <v>581</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29" t="s">
@@ -7244,7 +7244,7 @@
         <v>581</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29" t="s">
@@ -7269,7 +7269,7 @@
         <v>581</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29" t="s">
@@ -7294,7 +7294,7 @@
         <v>581</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -7319,7 +7319,7 @@
         <v>581</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -7344,7 +7344,7 @@
         <v>581</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29" t="s">
@@ -7363,13 +7363,13 @@
     </row>
     <row r="71" spans="1:9" ht="45">
       <c r="A71" s="34" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B71" s="30" t="s">
         <v>581</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D71" s="34"/>
       <c r="E71" s="29" t="s">
@@ -7388,13 +7388,13 @@
     </row>
     <row r="72" spans="1:9" ht="30">
       <c r="A72" s="34" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B72" s="30" t="s">
         <v>581</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D72" s="34"/>
       <c r="E72" s="29" t="s">
@@ -7538,13 +7538,13 @@
     </row>
     <row r="78" spans="1:9" ht="30">
       <c r="A78" s="22" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B78" s="30" t="s">
         <v>581</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D78" s="34"/>
       <c r="E78" s="29" t="s">
@@ -7563,13 +7563,13 @@
     </row>
     <row r="79" spans="1:9" ht="30">
       <c r="A79" s="22" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B79" s="30" t="s">
         <v>581</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D79" s="34"/>
       <c r="E79" s="29" t="s">
@@ -7594,7 +7594,7 @@
         <v>581</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D80" s="29"/>
       <c r="E80" s="29" t="s">
@@ -7644,7 +7644,7 @@
         <v>581</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D82" s="29"/>
       <c r="E82" s="29" t="s">
@@ -7671,7 +7671,7 @@
         <v>582</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D83" s="29"/>
       <c r="E83" s="29" t="s">
@@ -7687,7 +7687,7 @@
         <v>17</v>
       </c>
       <c r="I83" s="20" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="45">
@@ -7800,13 +7800,13 @@
     </row>
     <row r="88" spans="1:9" ht="45">
       <c r="A88" s="34" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B88" s="30" t="s">
         <v>582</v>
       </c>
       <c r="C88" s="32" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D88" s="34"/>
       <c r="E88" s="34" t="s">
@@ -7833,7 +7833,7 @@
         <v>583</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29" t="s">
@@ -7935,7 +7935,7 @@
         <v>584</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="29" t="s">
@@ -8037,7 +8037,7 @@
         <v>585</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D97" s="29"/>
       <c r="E97" s="29" t="s">
@@ -8166,7 +8166,7 @@
         <v>586</v>
       </c>
       <c r="C102" s="32" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="29" t="s">
@@ -8214,13 +8214,13 @@
     </row>
     <row r="104" spans="1:9" ht="60">
       <c r="A104" s="22" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B104" s="24" t="s">
         <v>586</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D104" s="34"/>
       <c r="E104" s="34" t="s">
@@ -8236,7 +8236,7 @@
         <v>17</v>
       </c>
       <c r="I104" s="32" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="30">
@@ -8405,7 +8405,7 @@
         <v>588</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D111" s="29"/>
       <c r="E111" s="29" t="s">
@@ -8655,13 +8655,13 @@
     </row>
     <row r="121" spans="1:9" ht="30">
       <c r="A121" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B121" s="30" t="s">
         <v>589</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D121" s="34"/>
       <c r="E121" s="29" t="s">
@@ -8680,13 +8680,13 @@
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="22" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B122" s="30" t="s">
         <v>589</v>
       </c>
       <c r="C122" s="32" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D122" s="34"/>
       <c r="E122" s="29" t="s">
@@ -8705,13 +8705,13 @@
     </row>
     <row r="123" spans="1:9" ht="30">
       <c r="A123" s="22" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B123" s="30" t="s">
         <v>589</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D123" s="34"/>
       <c r="E123" s="29" t="s">
@@ -8730,13 +8730,13 @@
     </row>
     <row r="124" spans="1:9" ht="30">
       <c r="A124" s="22" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B124" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D124" s="34"/>
       <c r="E124" s="29" t="s">
@@ -8758,10 +8758,10 @@
         <v>137</v>
       </c>
       <c r="B125" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C125" s="20" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29" t="s">
@@ -8785,10 +8785,10 @@
         <v>138</v>
       </c>
       <c r="B126" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="29" t="s">
@@ -8812,10 +8812,10 @@
         <v>139</v>
       </c>
       <c r="B127" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C127" s="20" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="29" t="s">
@@ -8837,10 +8837,10 @@
         <v>140</v>
       </c>
       <c r="B128" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="29" t="s">
@@ -8864,10 +8864,10 @@
         <v>141</v>
       </c>
       <c r="B129" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="29" t="s">
@@ -8889,10 +8889,10 @@
         <v>142</v>
       </c>
       <c r="B130" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="29" t="s">
@@ -8916,10 +8916,10 @@
         <v>143</v>
       </c>
       <c r="B131" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -8941,10 +8941,10 @@
         <v>144</v>
       </c>
       <c r="B132" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="29" t="s">
@@ -8966,10 +8966,10 @@
         <v>145</v>
       </c>
       <c r="B133" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D133" s="29"/>
       <c r="E133" s="29" t="s">
@@ -8991,10 +8991,10 @@
         <v>146</v>
       </c>
       <c r="B134" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="29" t="s">
@@ -9016,10 +9016,10 @@
         <v>147</v>
       </c>
       <c r="B135" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C135" s="20" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="29" t="s">
@@ -9041,10 +9041,10 @@
         <v>148</v>
       </c>
       <c r="B136" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C136" s="20" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="29" t="s">
@@ -9066,10 +9066,10 @@
         <v>149</v>
       </c>
       <c r="B137" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C137" s="20" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="29" t="s">
@@ -9091,10 +9091,10 @@
         <v>150</v>
       </c>
       <c r="B138" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29" t="s">
@@ -9116,10 +9116,10 @@
         <v>151</v>
       </c>
       <c r="B139" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="29" t="s">
@@ -9138,13 +9138,13 @@
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="22" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B140" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C140" s="32" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D140" s="34"/>
       <c r="E140" s="29" t="s">
@@ -9163,13 +9163,13 @@
     </row>
     <row r="141" spans="1:9" ht="30">
       <c r="A141" s="22" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B141" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C141" s="32" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D141" s="34"/>
       <c r="E141" s="29" t="s">
@@ -9188,13 +9188,13 @@
     </row>
     <row r="142" spans="1:9" ht="30">
       <c r="A142" s="22" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B142" s="35" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C142" s="32" t="s">
         <v>1099</v>
-      </c>
-      <c r="B142" s="35" t="s">
-        <v>1073</v>
-      </c>
-      <c r="C142" s="32" t="s">
-        <v>1100</v>
       </c>
       <c r="D142" s="34"/>
       <c r="E142" s="29" t="s">
@@ -9216,10 +9216,10 @@
         <v>152</v>
       </c>
       <c r="B143" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -9241,10 +9241,10 @@
         <v>153</v>
       </c>
       <c r="B144" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="29" t="s">
@@ -9266,10 +9266,10 @@
         <v>154</v>
       </c>
       <c r="B145" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D145" s="29"/>
       <c r="E145" s="29" t="s">
@@ -9291,10 +9291,10 @@
         <v>155</v>
       </c>
       <c r="B146" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C146" s="20" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="D146" s="29"/>
       <c r="E146" s="29" t="s">
@@ -9316,10 +9316,10 @@
         <v>156</v>
       </c>
       <c r="B147" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C147" s="20" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="D147" s="29"/>
       <c r="E147" s="29" t="s">
@@ -9341,10 +9341,10 @@
         <v>157</v>
       </c>
       <c r="B148" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C148" s="20" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D148" s="29"/>
       <c r="E148" s="29" t="s">
@@ -9366,10 +9366,10 @@
         <v>158</v>
       </c>
       <c r="B149" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C149" s="20" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="29" t="s">
@@ -9391,10 +9391,10 @@
         <v>159</v>
       </c>
       <c r="B150" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C150" s="20" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="29" t="s">
@@ -9418,10 +9418,10 @@
         <v>160</v>
       </c>
       <c r="B151" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C151" s="20" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="29" t="s">
@@ -9443,10 +9443,10 @@
         <v>161</v>
       </c>
       <c r="B152" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C152" s="20" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="29" t="s">
@@ -9468,10 +9468,10 @@
         <v>162</v>
       </c>
       <c r="B153" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C153" s="20" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
@@ -9495,10 +9495,10 @@
         <v>163</v>
       </c>
       <c r="B154" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C154" s="20" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="29" t="s">
@@ -9522,10 +9522,10 @@
         <v>164</v>
       </c>
       <c r="B155" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C155" s="20" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="29" t="s">
@@ -9547,10 +9547,10 @@
         <v>165</v>
       </c>
       <c r="B156" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C156" s="20" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="29" t="s">
@@ -9574,10 +9574,10 @@
         <v>166</v>
       </c>
       <c r="B157" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C157" s="20" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D157" s="29" t="s">
         <v>886</v>
@@ -9601,10 +9601,10 @@
         <v>167</v>
       </c>
       <c r="B158" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C158" s="20" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D158" s="29" t="s">
         <v>886</v>
@@ -9628,10 +9628,10 @@
         <v>168</v>
       </c>
       <c r="B159" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C159" s="20" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="D159" s="29"/>
       <c r="E159" s="29" t="s">
@@ -9655,10 +9655,10 @@
         <v>169</v>
       </c>
       <c r="B160" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C160" s="20" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D160" s="29"/>
       <c r="E160" s="29" t="s">
@@ -9680,10 +9680,10 @@
         <v>170</v>
       </c>
       <c r="B161" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C161" s="20" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D161" s="29"/>
       <c r="E161" s="29" t="s">
@@ -9707,10 +9707,10 @@
         <v>171</v>
       </c>
       <c r="B162" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C162" s="20" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D162" s="29"/>
       <c r="E162" s="29" t="s">
@@ -9732,10 +9732,10 @@
         <v>172</v>
       </c>
       <c r="B163" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C163" s="20" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D163" s="29"/>
       <c r="E163" s="29" t="s">
@@ -9757,10 +9757,10 @@
         <v>173</v>
       </c>
       <c r="B164" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C164" s="20" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="29" t="s">
@@ -9782,10 +9782,10 @@
         <v>174</v>
       </c>
       <c r="B165" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C165" s="20" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -9809,10 +9809,10 @@
         <v>175</v>
       </c>
       <c r="B166" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C166" s="20" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D166" s="29" t="s">
         <v>887</v>
@@ -9838,10 +9838,10 @@
         <v>176</v>
       </c>
       <c r="B167" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C167" s="20" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D167" s="29"/>
       <c r="E167" s="29" t="s">
@@ -9863,10 +9863,10 @@
         <v>177</v>
       </c>
       <c r="B168" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C168" s="20" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D168" s="29"/>
       <c r="E168" s="29" t="s">
@@ -9888,10 +9888,10 @@
         <v>178</v>
       </c>
       <c r="B169" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C169" s="20" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D169" s="29"/>
       <c r="E169" s="29" t="s">
@@ -9915,10 +9915,10 @@
         <v>179</v>
       </c>
       <c r="B170" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C170" s="20" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D170" s="29" t="s">
         <v>888</v>
@@ -9942,10 +9942,10 @@
         <v>180</v>
       </c>
       <c r="B171" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C171" s="20" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D171" s="29" t="s">
         <v>888</v>
@@ -9969,10 +9969,10 @@
         <v>181</v>
       </c>
       <c r="B172" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C172" s="20" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D172" s="29" t="s">
         <v>888</v>
@@ -9996,10 +9996,10 @@
         <v>182</v>
       </c>
       <c r="B173" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C173" s="20" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="D173" s="29" t="s">
         <v>888</v>
@@ -10023,10 +10023,10 @@
         <v>183</v>
       </c>
       <c r="B174" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C174" s="20" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="D174" s="29"/>
       <c r="E174" s="29" t="s">
@@ -10048,10 +10048,10 @@
         <v>184</v>
       </c>
       <c r="B175" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C175" s="20" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="29" t="s">
@@ -10073,10 +10073,10 @@
         <v>185</v>
       </c>
       <c r="B176" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C176" s="20" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D176" s="29"/>
       <c r="E176" s="29" t="s">
@@ -10100,10 +10100,10 @@
         <v>186</v>
       </c>
       <c r="B177" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C177" s="20" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="D177" s="29" t="s">
         <v>889</v>
@@ -10127,10 +10127,10 @@
         <v>187</v>
       </c>
       <c r="B178" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C178" s="20" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D178" s="29" t="s">
         <v>889</v>
@@ -10154,10 +10154,10 @@
         <v>188</v>
       </c>
       <c r="B179" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C179" s="20" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="D179" s="29" t="s">
         <v>889</v>
@@ -10181,10 +10181,10 @@
         <v>189</v>
       </c>
       <c r="B180" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C180" s="20" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D180" s="29" t="s">
         <v>889</v>
@@ -10208,10 +10208,10 @@
         <v>190</v>
       </c>
       <c r="B181" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C181" s="20" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D181" s="29"/>
       <c r="E181" s="29" t="s">
@@ -10233,10 +10233,10 @@
         <v>191</v>
       </c>
       <c r="B182" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C182" s="20" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D182" s="29"/>
       <c r="E182" s="29" t="s">
@@ -10258,10 +10258,10 @@
         <v>192</v>
       </c>
       <c r="B183" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C183" s="20" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D183" s="29"/>
       <c r="E183" s="29" t="s">
@@ -10285,10 +10285,10 @@
         <v>193</v>
       </c>
       <c r="B184" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C184" s="20" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D184" s="29" t="s">
         <v>890</v>
@@ -10312,10 +10312,10 @@
         <v>194</v>
       </c>
       <c r="B185" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C185" s="20" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="D185" s="29" t="s">
         <v>890</v>
@@ -10339,10 +10339,10 @@
         <v>195</v>
       </c>
       <c r="B186" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C186" s="20" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D186" s="29" t="s">
         <v>890</v>
@@ -10366,10 +10366,10 @@
         <v>196</v>
       </c>
       <c r="B187" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C187" s="20" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="D187" s="29" t="s">
         <v>890</v>
@@ -10393,10 +10393,10 @@
         <v>197</v>
       </c>
       <c r="B188" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C188" s="20" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="29" t="s">
@@ -10418,10 +10418,10 @@
         <v>198</v>
       </c>
       <c r="B189" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C189" s="20" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D189" s="29"/>
       <c r="E189" s="29" t="s">
@@ -10443,10 +10443,10 @@
         <v>199</v>
       </c>
       <c r="B190" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C190" s="20" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="D190" s="29"/>
       <c r="E190" s="29" t="s">
@@ -10470,10 +10470,10 @@
         <v>200</v>
       </c>
       <c r="B191" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C191" s="20" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D191" s="29" t="s">
         <v>891</v>
@@ -10497,10 +10497,10 @@
         <v>201</v>
       </c>
       <c r="B192" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C192" s="20" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D192" s="29" t="s">
         <v>891</v>
@@ -10524,10 +10524,10 @@
         <v>202</v>
       </c>
       <c r="B193" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C193" s="20" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D193" s="29" t="s">
         <v>891</v>
@@ -10551,10 +10551,10 @@
         <v>203</v>
       </c>
       <c r="B194" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C194" s="20" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="29" t="s">
@@ -10576,10 +10576,10 @@
         <v>204</v>
       </c>
       <c r="B195" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C195" s="20" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D195" s="29"/>
       <c r="E195" s="29" t="s">
@@ -10601,10 +10601,10 @@
         <v>205</v>
       </c>
       <c r="B196" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C196" s="20" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -10628,10 +10628,10 @@
         <v>206</v>
       </c>
       <c r="B197" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C197" s="20" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="D197" s="29" t="s">
         <v>892</v>
@@ -10655,10 +10655,10 @@
         <v>207</v>
       </c>
       <c r="B198" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="D198" s="29" t="s">
         <v>892</v>
@@ -10682,10 +10682,10 @@
         <v>208</v>
       </c>
       <c r="B199" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C199" s="20" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="D199" s="29" t="s">
         <v>892</v>
@@ -10709,10 +10709,10 @@
         <v>209</v>
       </c>
       <c r="B200" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C200" s="20" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="D200" s="29"/>
       <c r="E200" s="29" t="s">
@@ -10734,10 +10734,10 @@
         <v>210</v>
       </c>
       <c r="B201" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -10756,16 +10756,16 @@
     </row>
     <row r="202" spans="1:9" ht="75">
       <c r="A202" s="34" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B202" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C202" s="32" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D202" s="22" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="E202" s="29" t="s">
         <v>19</v>
@@ -10780,21 +10780,21 @@
         <v>17</v>
       </c>
       <c r="I202" s="32" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="203" spans="1:9" ht="45">
       <c r="A203" s="34" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B203" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C203" s="32" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D203" s="22" t="s">
         <v>1167</v>
-      </c>
-      <c r="D203" s="22" t="s">
-        <v>1168</v>
       </c>
       <c r="E203" s="29" t="s">
         <v>19</v>
@@ -10812,16 +10812,16 @@
     </row>
     <row r="204" spans="1:9" ht="45">
       <c r="A204" s="34" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B204" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C204" s="32" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="D204" s="22" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="E204" s="29" t="s">
         <v>19</v>
@@ -10839,16 +10839,16 @@
     </row>
     <row r="205" spans="1:9" ht="30">
       <c r="A205" s="34" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B205" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C205" s="32" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="D205" s="22" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="E205" s="29" t="s">
         <v>19</v>
@@ -10869,10 +10869,10 @@
         <v>211</v>
       </c>
       <c r="B206" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C206" s="20" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="D206" s="29"/>
       <c r="E206" s="29" t="s">
@@ -10894,10 +10894,10 @@
         <v>212</v>
       </c>
       <c r="B207" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C207" s="20" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="D207" s="29"/>
       <c r="E207" s="29" t="s">
@@ -10919,10 +10919,10 @@
         <v>213</v>
       </c>
       <c r="B208" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C208" s="20" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -10946,10 +10946,10 @@
         <v>214</v>
       </c>
       <c r="B209" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C209" s="20" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="D209" s="29" t="s">
         <v>893</v>
@@ -10973,10 +10973,10 @@
         <v>215</v>
       </c>
       <c r="B210" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C210" s="20" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="D210" s="29" t="s">
         <v>893</v>
@@ -11000,10 +11000,10 @@
         <v>216</v>
       </c>
       <c r="B211" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C211" s="20" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="D211" s="29" t="s">
         <v>893</v>
@@ -11027,10 +11027,10 @@
         <v>217</v>
       </c>
       <c r="B212" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C212" s="20" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D212" s="29"/>
       <c r="E212" s="29" t="s">
@@ -11049,13 +11049,13 @@
     </row>
     <row r="213" spans="1:9" ht="30">
       <c r="A213" s="22" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B213" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C213" s="32" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D213" s="34"/>
       <c r="E213" s="34" t="s">
@@ -11077,10 +11077,10 @@
         <v>218</v>
       </c>
       <c r="B214" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C214" s="20" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="D214" s="29"/>
       <c r="E214" s="29" t="s">
@@ -11104,10 +11104,10 @@
         <v>219</v>
       </c>
       <c r="B215" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C215" s="20" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="D215" s="29" t="s">
         <v>894</v>
@@ -11131,10 +11131,10 @@
         <v>220</v>
       </c>
       <c r="B216" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C216" s="20" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="D216" s="29" t="s">
         <v>894</v>
@@ -11158,10 +11158,10 @@
         <v>221</v>
       </c>
       <c r="B217" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C217" s="20" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D217" s="29" t="s">
         <v>894</v>
@@ -11185,10 +11185,10 @@
         <v>222</v>
       </c>
       <c r="B218" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C218" s="20" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="D218" s="29"/>
       <c r="E218" s="29" t="s">
@@ -11210,10 +11210,10 @@
         <v>223</v>
       </c>
       <c r="B219" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C219" s="20" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D219" s="29"/>
       <c r="E219" s="29" t="s">
@@ -11235,10 +11235,10 @@
         <v>224</v>
       </c>
       <c r="B220" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C220" s="20" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D220" s="29"/>
       <c r="E220" s="29" t="s">
@@ -11262,10 +11262,10 @@
         <v>225</v>
       </c>
       <c r="B221" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C221" s="20" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D221" s="29" t="s">
         <v>895</v>
@@ -11289,10 +11289,10 @@
         <v>226</v>
       </c>
       <c r="B222" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C222" s="20" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D222" s="29" t="s">
         <v>895</v>
@@ -11316,10 +11316,10 @@
         <v>227</v>
       </c>
       <c r="B223" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C223" s="20" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="D223" s="29" t="s">
         <v>895</v>
@@ -11343,10 +11343,10 @@
         <v>228</v>
       </c>
       <c r="B224" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C224" s="20" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D224" s="29"/>
       <c r="E224" s="29" t="s">
@@ -11368,10 +11368,10 @@
         <v>229</v>
       </c>
       <c r="B225" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C225" s="20" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D225" s="29"/>
       <c r="E225" s="29" t="s">
@@ -11393,10 +11393,10 @@
         <v>230</v>
       </c>
       <c r="B226" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C226" s="20" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="D226" s="29"/>
       <c r="E226" s="29" t="s">
@@ -11420,10 +11420,10 @@
         <v>231</v>
       </c>
       <c r="B227" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C227" s="20" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="D227" s="29" t="s">
         <v>896</v>
@@ -11447,10 +11447,10 @@
         <v>232</v>
       </c>
       <c r="B228" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C228" s="20" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="D228" s="29" t="s">
         <v>896</v>
@@ -11474,10 +11474,10 @@
         <v>233</v>
       </c>
       <c r="B229" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C229" s="20" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="D229" s="29" t="s">
         <v>896</v>
@@ -11501,10 +11501,10 @@
         <v>234</v>
       </c>
       <c r="B230" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C230" s="20" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D230" s="29"/>
       <c r="E230" s="29" t="s">
@@ -11526,10 +11526,10 @@
         <v>235</v>
       </c>
       <c r="B231" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C231" s="20" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="D231" s="29"/>
       <c r="E231" s="29" t="s">
@@ -11551,10 +11551,10 @@
         <v>236</v>
       </c>
       <c r="B232" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C232" s="20" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D232" s="29"/>
       <c r="E232" s="29" t="s">
@@ -11578,10 +11578,10 @@
         <v>237</v>
       </c>
       <c r="B233" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C233" s="20" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="D233" s="29" t="s">
         <v>897</v>
@@ -11605,10 +11605,10 @@
         <v>238</v>
       </c>
       <c r="B234" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C234" s="20" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D234" s="29" t="s">
         <v>897</v>
@@ -11632,10 +11632,10 @@
         <v>239</v>
       </c>
       <c r="B235" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C235" s="20" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="D235" s="29" t="s">
         <v>897</v>
@@ -11659,10 +11659,10 @@
         <v>240</v>
       </c>
       <c r="B236" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C236" s="20" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="D236" s="29" t="s">
         <v>897</v>
@@ -11686,10 +11686,10 @@
         <v>241</v>
       </c>
       <c r="B237" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C237" s="20" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="D237" s="29" t="s">
         <v>897</v>
@@ -11713,10 +11713,10 @@
         <v>242</v>
       </c>
       <c r="B238" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C238" s="20" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="D238" s="29"/>
       <c r="E238" s="29" t="s">
@@ -11738,10 +11738,10 @@
         <v>243</v>
       </c>
       <c r="B239" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C239" s="20" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="D239" s="29"/>
       <c r="E239" s="29" t="s">
@@ -11763,10 +11763,10 @@
         <v>244</v>
       </c>
       <c r="B240" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C240" s="20" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="D240" s="29"/>
       <c r="E240" s="29" t="s">
@@ -11790,10 +11790,10 @@
         <v>245</v>
       </c>
       <c r="B241" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C241" s="20" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D241" s="29" t="s">
         <v>898</v>
@@ -11817,10 +11817,10 @@
         <v>246</v>
       </c>
       <c r="B242" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C242" s="20" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="D242" s="29" t="s">
         <v>898</v>
@@ -11844,10 +11844,10 @@
         <v>247</v>
       </c>
       <c r="B243" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C243" s="20" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D243" s="29" t="s">
         <v>898</v>
@@ -11871,10 +11871,10 @@
         <v>248</v>
       </c>
       <c r="B244" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C244" s="20" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="D244" s="29"/>
       <c r="E244" s="29" t="s">
@@ -11896,10 +11896,10 @@
         <v>249</v>
       </c>
       <c r="B245" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C245" s="20" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="D245" s="29"/>
       <c r="E245" s="29" t="s">
@@ -11921,10 +11921,10 @@
         <v>250</v>
       </c>
       <c r="B246" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C246" s="20" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="D246" s="29"/>
       <c r="E246" s="29" t="s">
@@ -11948,10 +11948,10 @@
         <v>251</v>
       </c>
       <c r="B247" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C247" s="20" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="D247" s="29" t="s">
         <v>899</v>
@@ -11975,10 +11975,10 @@
         <v>252</v>
       </c>
       <c r="B248" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C248" s="20" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D248" s="29" t="s">
         <v>899</v>
@@ -12002,10 +12002,10 @@
         <v>253</v>
       </c>
       <c r="B249" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C249" s="20" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D249" s="29" t="s">
         <v>899</v>
@@ -12029,10 +12029,10 @@
         <v>254</v>
       </c>
       <c r="B250" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C250" s="20" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="D250" s="29"/>
       <c r="E250" s="29" t="s">
@@ -12054,10 +12054,10 @@
         <v>255</v>
       </c>
       <c r="B251" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C251" s="20" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="D251" s="29"/>
       <c r="E251" s="29" t="s">
@@ -12079,10 +12079,10 @@
         <v>256</v>
       </c>
       <c r="B252" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C252" s="20" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="D252" s="29"/>
       <c r="E252" s="29" t="s">
@@ -12106,10 +12106,10 @@
         <v>257</v>
       </c>
       <c r="B253" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C253" s="20" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D253" s="29" t="s">
         <v>900</v>
@@ -12133,10 +12133,10 @@
         <v>258</v>
       </c>
       <c r="B254" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C254" s="20" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D254" s="29" t="s">
         <v>900</v>
@@ -12160,10 +12160,10 @@
         <v>259</v>
       </c>
       <c r="B255" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C255" s="20" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="D255" s="29" t="s">
         <v>900</v>
@@ -12187,10 +12187,10 @@
         <v>260</v>
       </c>
       <c r="B256" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C256" s="20" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="D256" s="29"/>
       <c r="E256" s="29" t="s">
@@ -12212,10 +12212,10 @@
         <v>261</v>
       </c>
       <c r="B257" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C257" s="20" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="D257" s="29"/>
       <c r="E257" s="29" t="s">
@@ -12237,10 +12237,10 @@
         <v>262</v>
       </c>
       <c r="B258" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C258" s="20" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D258" s="29"/>
       <c r="E258" s="29" t="s">
@@ -12264,10 +12264,10 @@
         <v>263</v>
       </c>
       <c r="B259" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C259" s="20" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="D259" s="29" t="s">
         <v>901</v>
@@ -12291,10 +12291,10 @@
         <v>264</v>
       </c>
       <c r="B260" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C260" s="20" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D260" s="29" t="s">
         <v>901</v>
@@ -12318,10 +12318,10 @@
         <v>265</v>
       </c>
       <c r="B261" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C261" s="20" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="D261" s="29" t="s">
         <v>901</v>
@@ -12345,10 +12345,10 @@
         <v>266</v>
       </c>
       <c r="B262" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C262" s="20" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D262" s="29"/>
       <c r="E262" s="29" t="s">
@@ -12372,10 +12372,10 @@
         <v>267</v>
       </c>
       <c r="B263" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C263" s="20" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="D263" s="29"/>
       <c r="E263" s="29" t="s">
@@ -12397,10 +12397,10 @@
         <v>268</v>
       </c>
       <c r="B264" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C264" s="20" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="D264" s="29"/>
       <c r="E264" s="29" t="s">
@@ -12422,10 +12422,10 @@
         <v>269</v>
       </c>
       <c r="B265" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C265" s="20" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="D265" s="29" t="s">
         <v>902</v>
@@ -12449,10 +12449,10 @@
         <v>270</v>
       </c>
       <c r="B266" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C266" s="20" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="D266" s="29" t="s">
         <v>902</v>
@@ -12476,10 +12476,10 @@
         <v>271</v>
       </c>
       <c r="B267" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C267" s="20" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="D267" s="29" t="s">
         <v>902</v>
@@ -12503,10 +12503,10 @@
         <v>272</v>
       </c>
       <c r="B268" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C268" s="20" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="D268" s="29"/>
       <c r="E268" s="29" t="s">
@@ -12528,10 +12528,10 @@
         <v>273</v>
       </c>
       <c r="B269" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C269" s="20" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="D269" s="29"/>
       <c r="E269" s="29" t="s">
@@ -12553,10 +12553,10 @@
         <v>274</v>
       </c>
       <c r="B270" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C270" s="20" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="D270" s="29"/>
       <c r="E270" s="29" t="s">
@@ -12578,10 +12578,10 @@
         <v>275</v>
       </c>
       <c r="B271" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C271" s="20" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="D271" s="29" t="s">
         <v>903</v>
@@ -12605,10 +12605,10 @@
         <v>276</v>
       </c>
       <c r="B272" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C272" s="20" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="D272" s="29" t="s">
         <v>903</v>
@@ -12632,10 +12632,10 @@
         <v>277</v>
       </c>
       <c r="B273" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C273" s="20" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="D273" s="29"/>
       <c r="E273" s="29" t="s">
@@ -12657,10 +12657,10 @@
         <v>278</v>
       </c>
       <c r="B274" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C274" s="20" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="D274" s="29"/>
       <c r="E274" s="29" t="s">
@@ -12682,10 +12682,10 @@
         <v>279</v>
       </c>
       <c r="B275" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C275" s="20" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="D275" s="29"/>
       <c r="E275" s="29" t="s">
@@ -12707,10 +12707,10 @@
         <v>280</v>
       </c>
       <c r="B276" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C276" s="20" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="D276" s="29" t="s">
         <v>904</v>
@@ -12734,10 +12734,10 @@
         <v>281</v>
       </c>
       <c r="B277" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C277" s="20" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="D277" s="29" t="s">
         <v>904</v>
@@ -12761,10 +12761,10 @@
         <v>282</v>
       </c>
       <c r="B278" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C278" s="20" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="D278" s="29"/>
       <c r="E278" s="29" t="s">
@@ -12786,10 +12786,10 @@
         <v>283</v>
       </c>
       <c r="B279" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C279" s="20" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="D279" s="29"/>
       <c r="E279" s="29" t="s">
@@ -12805,7 +12805,7 @@
         <v>17</v>
       </c>
       <c r="I279" s="20" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="280" spans="1:9" ht="60">
@@ -12813,10 +12813,10 @@
         <v>284</v>
       </c>
       <c r="B280" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C280" s="20" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="D280" s="29"/>
       <c r="E280" s="29" t="s">
@@ -12840,10 +12840,10 @@
         <v>285</v>
       </c>
       <c r="B281" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C281" s="20" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="D281" s="29" t="s">
         <v>905</v>
@@ -12867,10 +12867,10 @@
         <v>286</v>
       </c>
       <c r="B282" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C282" s="20" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="D282" s="29" t="s">
         <v>905</v>
@@ -12894,10 +12894,10 @@
         <v>287</v>
       </c>
       <c r="B283" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C283" s="20" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="D283" s="29"/>
       <c r="E283" s="29" t="s">
@@ -12919,10 +12919,10 @@
         <v>288</v>
       </c>
       <c r="B284" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C284" s="20" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="D284" s="29"/>
       <c r="E284" s="29" t="s">
@@ -12944,10 +12944,10 @@
         <v>289</v>
       </c>
       <c r="B285" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C285" s="20" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="D285" s="29"/>
       <c r="E285" s="29" t="s">
@@ -12969,10 +12969,10 @@
         <v>290</v>
       </c>
       <c r="B286" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C286" s="20" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="D286" s="29"/>
       <c r="E286" s="29" t="s">
@@ -12994,10 +12994,10 @@
         <v>291</v>
       </c>
       <c r="B287" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C287" s="20" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="D287" s="29"/>
       <c r="E287" s="29" t="s">
@@ -13021,10 +13021,10 @@
         <v>292</v>
       </c>
       <c r="B288" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C288" s="20" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="D288" s="29" t="s">
         <v>906</v>
@@ -13048,10 +13048,10 @@
         <v>293</v>
       </c>
       <c r="B289" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C289" s="20" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="D289" s="29" t="s">
         <v>906</v>
@@ -13075,10 +13075,10 @@
         <v>294</v>
       </c>
       <c r="B290" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C290" s="20" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D290" s="29"/>
       <c r="E290" s="29" t="s">
@@ -13100,10 +13100,10 @@
         <v>295</v>
       </c>
       <c r="B291" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C291" s="20" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D291" s="29"/>
       <c r="E291" s="29" t="s">
@@ -13125,10 +13125,10 @@
         <v>296</v>
       </c>
       <c r="B292" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C292" s="20" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="D292" s="29"/>
       <c r="E292" s="29" t="s">
@@ -13150,10 +13150,10 @@
         <v>297</v>
       </c>
       <c r="B293" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C293" s="20" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="D293" s="29"/>
       <c r="E293" s="29" t="s">
@@ -13177,10 +13177,10 @@
         <v>298</v>
       </c>
       <c r="B294" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C294" s="20" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="D294" s="29" t="s">
         <v>907</v>
@@ -13204,10 +13204,10 @@
         <v>299</v>
       </c>
       <c r="B295" s="35" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C295" s="20" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="D295" s="29" t="s">
         <v>907</v>
@@ -13334,7 +13334,7 @@
         <v>590</v>
       </c>
       <c r="C300" s="20" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="D300" s="29"/>
       <c r="E300" s="29" t="s">
@@ -13463,7 +13463,7 @@
         <v>32</v>
       </c>
       <c r="C305" s="20" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="D305" s="29"/>
       <c r="E305" s="29" t="s">
@@ -13613,7 +13613,7 @@
         <v>592</v>
       </c>
       <c r="C311" s="20" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="D311" s="29"/>
       <c r="E311" s="29" t="s">
@@ -14200,7 +14200,7 @@
         <v>592</v>
       </c>
       <c r="C334" s="20" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="D334" s="29"/>
       <c r="E334" s="29" t="s">
@@ -14225,7 +14225,7 @@
         <v>592</v>
       </c>
       <c r="C335" s="20" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="D335" s="29"/>
       <c r="E335" s="29" t="s">
@@ -14250,7 +14250,7 @@
         <v>592</v>
       </c>
       <c r="C336" s="20" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="D336" s="29"/>
       <c r="E336" s="29" t="s">
@@ -14277,7 +14277,7 @@
         <v>592</v>
       </c>
       <c r="C337" s="20" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="D337" s="29"/>
       <c r="E337" s="29" t="s">
@@ -14304,7 +14304,7 @@
         <v>592</v>
       </c>
       <c r="C338" s="20" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="D338" s="29"/>
       <c r="E338" s="29" t="s">
@@ -14331,7 +14331,7 @@
         <v>592</v>
       </c>
       <c r="C339" s="20" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="D339" s="29"/>
       <c r="E339" s="29" t="s">
@@ -14358,7 +14358,7 @@
         <v>592</v>
       </c>
       <c r="C340" s="20" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="D340" s="29"/>
       <c r="E340" s="29" t="s">
@@ -14385,7 +14385,7 @@
         <v>592</v>
       </c>
       <c r="C341" s="20" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="D341" s="29"/>
       <c r="E341" s="29" t="s">
@@ -14410,7 +14410,7 @@
         <v>592</v>
       </c>
       <c r="C342" s="20" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="D342" s="29"/>
       <c r="E342" s="29" t="s">
@@ -14543,7 +14543,7 @@
         <v>594</v>
       </c>
       <c r="C347" s="20" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="D347" s="29"/>
       <c r="E347" s="29" t="s">
@@ -14620,7 +14620,7 @@
         <v>595</v>
       </c>
       <c r="C350" s="20" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="D350" s="29"/>
       <c r="E350" s="29" t="s">
@@ -14742,7 +14742,7 @@
         <v>17</v>
       </c>
       <c r="I354" s="20" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="355" spans="1:9" ht="45">
@@ -14803,7 +14803,7 @@
         <v>596</v>
       </c>
       <c r="C357" s="20" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="D357" s="29"/>
       <c r="E357" s="29" t="s">
@@ -15144,7 +15144,7 @@
         <v>597</v>
       </c>
       <c r="C370" s="20" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="D370" s="29"/>
       <c r="E370" s="29" t="s">
@@ -15221,7 +15221,7 @@
         <v>598</v>
       </c>
       <c r="C373" s="20" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="D373" s="29"/>
       <c r="E373" s="29" t="s">
@@ -15479,7 +15479,7 @@
         <v>604</v>
       </c>
       <c r="C383" s="20" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="D383" s="29"/>
       <c r="E383" s="29" t="s">
@@ -15504,7 +15504,7 @@
         <v>604</v>
       </c>
       <c r="C384" s="20" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="D384" s="29"/>
       <c r="E384" s="29" t="s">
@@ -15529,7 +15529,7 @@
         <v>604</v>
       </c>
       <c r="C385" s="20" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="D385" s="29"/>
       <c r="E385" s="29" t="s">
@@ -15554,7 +15554,7 @@
         <v>604</v>
       </c>
       <c r="C386" s="20" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="D386" s="29"/>
       <c r="E386" s="29" t="s">
@@ -15579,7 +15579,7 @@
         <v>604</v>
       </c>
       <c r="C387" s="20" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="D387" s="29"/>
       <c r="E387" s="29" t="s">
@@ -15604,7 +15604,7 @@
         <v>604</v>
       </c>
       <c r="C388" s="20" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D388" s="29"/>
       <c r="E388" s="29" t="s">
@@ -15629,7 +15629,7 @@
         <v>604</v>
       </c>
       <c r="C389" s="20" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="D389" s="29"/>
       <c r="E389" s="29" t="s">
@@ -15654,7 +15654,7 @@
         <v>604</v>
       </c>
       <c r="C390" s="20" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="D390" s="29"/>
       <c r="E390" s="29" t="s">
@@ -15679,7 +15679,7 @@
         <v>604</v>
       </c>
       <c r="C391" s="20" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="D391" s="29"/>
       <c r="E391" s="29" t="s">
@@ -15754,7 +15754,7 @@
         <v>604</v>
       </c>
       <c r="C394" s="20" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="D394" s="29"/>
       <c r="E394" s="29" t="s">
@@ -15779,7 +15779,7 @@
         <v>604</v>
       </c>
       <c r="C395" s="20" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="D395" s="29"/>
       <c r="E395" s="29" t="s">
@@ -15804,7 +15804,7 @@
         <v>604</v>
       </c>
       <c r="C396" s="20" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="D396" s="29"/>
       <c r="E396" s="29" t="s">
@@ -15829,7 +15829,7 @@
         <v>604</v>
       </c>
       <c r="C397" s="20" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="D397" s="29"/>
       <c r="E397" s="29" t="s">
@@ -15854,7 +15854,7 @@
         <v>604</v>
       </c>
       <c r="C398" s="20" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="D398" s="29"/>
       <c r="E398" s="29" t="s">
@@ -15879,7 +15879,7 @@
         <v>604</v>
       </c>
       <c r="C399" s="20" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="D399" s="29"/>
       <c r="E399" s="29" t="s">
@@ -15904,7 +15904,7 @@
         <v>604</v>
       </c>
       <c r="C400" s="20" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="D400" s="29"/>
       <c r="E400" s="29" t="s">
@@ -15929,7 +15929,7 @@
         <v>604</v>
       </c>
       <c r="C401" s="20" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="D401" s="29"/>
       <c r="E401" s="29" t="s">
@@ -15954,7 +15954,7 @@
         <v>604</v>
       </c>
       <c r="C402" s="20" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="D402" s="29"/>
       <c r="E402" s="29" t="s">
@@ -15979,7 +15979,7 @@
         <v>605</v>
       </c>
       <c r="C403" s="20" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="D403" s="29"/>
       <c r="E403" s="29" t="s">
@@ -16054,7 +16054,7 @@
         <v>606</v>
       </c>
       <c r="C406" s="20" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="D406" s="29"/>
       <c r="E406" s="29" t="s">
@@ -16179,7 +16179,7 @@
         <v>607</v>
       </c>
       <c r="C411" s="20" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="D411" s="29"/>
       <c r="E411" s="29" t="s">
@@ -16329,7 +16329,7 @@
         <v>607</v>
       </c>
       <c r="C417" s="20" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="D417" s="29"/>
       <c r="E417" s="29" t="s">
@@ -16754,7 +16754,7 @@
         <v>612</v>
       </c>
       <c r="C434" s="20" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="D434" s="29"/>
       <c r="E434" s="29" t="s">
@@ -16854,7 +16854,7 @@
         <v>612</v>
       </c>
       <c r="C438" s="20" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="D438" s="29"/>
       <c r="E438" s="29" t="s">
@@ -17229,7 +17229,7 @@
         <v>616</v>
       </c>
       <c r="C453" s="20" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="D453" s="29"/>
       <c r="E453" s="29" t="s">
@@ -17254,7 +17254,7 @@
         <v>616</v>
       </c>
       <c r="C454" s="20" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="D454" s="29"/>
       <c r="E454" s="29" t="s">
@@ -17279,7 +17279,7 @@
         <v>616</v>
       </c>
       <c r="C455" s="20" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="D455" s="29"/>
       <c r="E455" s="29" t="s">
@@ -17529,7 +17529,7 @@
         <v>618</v>
       </c>
       <c r="C465" s="20" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="D465" s="29"/>
       <c r="E465" s="29" t="s">
@@ -17912,7 +17912,7 @@
         <v>619</v>
       </c>
       <c r="C480" s="20" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="D480" s="29"/>
       <c r="E480" s="29" t="s">
@@ -17937,7 +17937,7 @@
         <v>619</v>
       </c>
       <c r="C481" s="20" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="D481" s="29" t="s">
         <v>909</v>
@@ -18095,7 +18095,7 @@
         <v>619</v>
       </c>
       <c r="C487" s="20" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="D487" s="29" t="s">
         <v>910</v>
@@ -18151,7 +18151,7 @@
         <v>619</v>
       </c>
       <c r="C489" s="20" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="D489" s="29" t="s">
         <v>911</v>
@@ -18263,7 +18263,7 @@
         <v>619</v>
       </c>
       <c r="C493" s="20" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="D493" s="29"/>
       <c r="E493" s="29" t="s">
@@ -18288,7 +18288,7 @@
         <v>619</v>
       </c>
       <c r="C494" s="20" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D494" s="29" t="s">
         <v>912</v>
@@ -18315,7 +18315,7 @@
         <v>619</v>
       </c>
       <c r="C495" s="20" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="D495" s="29" t="s">
         <v>912</v>
@@ -18342,7 +18342,7 @@
         <v>619</v>
       </c>
       <c r="C496" s="20" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="D496" s="29" t="s">
         <v>912</v>
@@ -18369,7 +18369,7 @@
         <v>619</v>
       </c>
       <c r="C497" s="20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="D497" s="29"/>
       <c r="E497" s="29" t="s">
@@ -18394,7 +18394,7 @@
         <v>619</v>
       </c>
       <c r="C498" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="D498" s="29" t="s">
         <v>912</v>
@@ -18415,16 +18415,16 @@
     </row>
     <row r="499" spans="1:9" ht="45">
       <c r="A499" s="34" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B499" s="35" t="s">
         <v>619</v>
       </c>
       <c r="C499" s="32" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="D499" s="34" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="E499" s="29" t="s">
         <v>22</v>
@@ -18442,13 +18442,13 @@
     </row>
     <row r="500" spans="1:9" ht="45">
       <c r="A500" s="34" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B500" s="35" t="s">
         <v>619</v>
       </c>
       <c r="C500" s="32" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="D500" s="34"/>
       <c r="E500" s="29" t="s">
@@ -18467,13 +18467,13 @@
     </row>
     <row r="501" spans="1:9" ht="45">
       <c r="A501" s="34" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B501" s="35" t="s">
         <v>619</v>
       </c>
       <c r="C501" s="32" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="D501" s="34"/>
       <c r="E501" s="29" t="s">
@@ -18492,16 +18492,16 @@
     </row>
     <row r="502" spans="1:9" ht="45">
       <c r="A502" s="34" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B502" s="35" t="s">
         <v>619</v>
       </c>
       <c r="C502" s="32" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="D502" s="34" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="E502" s="29" t="s">
         <v>22</v>
@@ -18521,13 +18521,13 @@
     </row>
     <row r="503" spans="1:9" ht="45">
       <c r="A503" s="22" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="B503" s="30" t="s">
         <v>619</v>
       </c>
       <c r="C503" s="20" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="D503" s="22" t="s">
         <v>1031</v>
@@ -18556,7 +18556,7 @@
         <v>619</v>
       </c>
       <c r="C504" s="20" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="D504" s="22" t="s">
         <v>1031</v>
@@ -18583,7 +18583,7 @@
         <v>619</v>
       </c>
       <c r="C505" s="20" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="D505" s="22" t="s">
         <v>1031</v>
@@ -18610,7 +18610,7 @@
         <v>619</v>
       </c>
       <c r="C506" s="20" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="D506" s="29"/>
       <c r="E506" s="29" t="s">
@@ -18635,7 +18635,7 @@
         <v>619</v>
       </c>
       <c r="C507" s="20" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="D507" s="29"/>
       <c r="E507" s="29" t="s">
@@ -18660,7 +18660,7 @@
         <v>619</v>
       </c>
       <c r="C508" s="20" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="D508" s="29"/>
       <c r="E508" s="29" t="s">
@@ -18685,7 +18685,7 @@
         <v>619</v>
       </c>
       <c r="C509" s="20" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="D509" s="29" t="s">
         <v>913</v>
@@ -18714,7 +18714,7 @@
         <v>619</v>
       </c>
       <c r="C510" s="20" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="D510" s="29" t="s">
         <v>913</v>
@@ -18741,7 +18741,7 @@
         <v>619</v>
       </c>
       <c r="C511" s="20" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="D511" s="29" t="s">
         <v>913</v>
@@ -18793,16 +18793,16 @@
     </row>
     <row r="513" spans="1:9" ht="45">
       <c r="A513" s="34" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B513" s="35" t="s">
         <v>619</v>
       </c>
       <c r="C513" s="32" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="D513" s="34" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="E513" s="29" t="s">
         <v>22</v>
@@ -18822,16 +18822,16 @@
     </row>
     <row r="514" spans="1:9" ht="45">
       <c r="A514" s="34" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B514" s="35" t="s">
         <v>619</v>
       </c>
       <c r="C514" s="32" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="D514" s="34" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="E514" s="29" t="s">
         <v>22</v>
@@ -18857,7 +18857,7 @@
         <v>619</v>
       </c>
       <c r="C515" s="20" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="D515" s="29"/>
       <c r="E515" s="29" t="s">
@@ -18882,7 +18882,7 @@
         <v>619</v>
       </c>
       <c r="C516" s="20" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="D516" s="29"/>
       <c r="E516" s="29" t="s">
@@ -18907,7 +18907,7 @@
         <v>619</v>
       </c>
       <c r="C517" s="20" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="D517" s="29"/>
       <c r="E517" s="29" t="s">
@@ -18932,7 +18932,7 @@
         <v>619</v>
       </c>
       <c r="C518" s="20" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="D518" s="29"/>
       <c r="E518" s="29" t="s">
@@ -18957,7 +18957,7 @@
         <v>619</v>
       </c>
       <c r="C519" s="20" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="D519" s="29"/>
       <c r="E519" s="29" t="s">
@@ -18982,7 +18982,7 @@
         <v>619</v>
       </c>
       <c r="C520" s="20" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D520" s="29"/>
       <c r="E520" s="29" t="s">
@@ -19009,7 +19009,7 @@
         <v>619</v>
       </c>
       <c r="C521" s="20" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="D521" s="29" t="s">
         <v>915</v>
@@ -19038,7 +19038,7 @@
         <v>619</v>
       </c>
       <c r="C522" s="20" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="D522" s="29" t="s">
         <v>915</v>
@@ -19181,7 +19181,7 @@
         <v>619</v>
       </c>
       <c r="C527" s="20" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D527" s="29" t="s">
         <v>919</v>
@@ -19210,7 +19210,7 @@
         <v>619</v>
       </c>
       <c r="C528" s="20" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="D528" s="29" t="s">
         <v>919</v>
@@ -19498,7 +19498,7 @@
         <v>619</v>
       </c>
       <c r="C538" s="20" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="D538" s="29" t="s">
         <v>928</v>
@@ -19554,7 +19554,7 @@
         <v>619</v>
       </c>
       <c r="C540" s="20" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="D540" s="29" t="s">
         <v>929</v>
@@ -19697,7 +19697,7 @@
         <v>619</v>
       </c>
       <c r="C545" s="20" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="D545" s="29" t="s">
         <v>932</v>
@@ -19778,7 +19778,7 @@
         <v>619</v>
       </c>
       <c r="C548" s="20" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="D548" s="29" t="s">
         <v>932</v>
@@ -20168,7 +20168,7 @@
         <v>619</v>
       </c>
       <c r="C562" s="20" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="D562" s="29"/>
       <c r="E562" s="29" t="s">
@@ -20195,7 +20195,7 @@
         <v>619</v>
       </c>
       <c r="C563" s="20" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="D563" s="29"/>
       <c r="E563" s="29" t="s">
@@ -20220,7 +20220,7 @@
         <v>619</v>
       </c>
       <c r="C564" s="20" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="D564" s="29"/>
       <c r="E564" s="29" t="s">
@@ -20245,7 +20245,7 @@
         <v>619</v>
       </c>
       <c r="C565" s="20" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="D565" s="29"/>
       <c r="E565" s="29" t="s">
@@ -20270,7 +20270,7 @@
         <v>619</v>
       </c>
       <c r="C566" s="20" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="D566" s="29"/>
       <c r="E566" s="29" t="s">
@@ -20353,7 +20353,7 @@
         <v>619</v>
       </c>
       <c r="C569" s="20" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="D569" s="29"/>
       <c r="E569" s="29" t="s">
@@ -20378,7 +20378,7 @@
         <v>619</v>
       </c>
       <c r="C570" s="20" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="D570" s="29"/>
       <c r="E570" s="29" t="s">
@@ -20403,7 +20403,7 @@
         <v>619</v>
       </c>
       <c r="C571" s="20" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="D571" s="29"/>
       <c r="E571" s="29" t="s">
@@ -20428,7 +20428,7 @@
         <v>619</v>
       </c>
       <c r="C572" s="20" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="D572" s="29"/>
       <c r="E572" s="29" t="s">
@@ -20453,7 +20453,7 @@
         <v>619</v>
       </c>
       <c r="C573" s="20" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="D573" s="29"/>
       <c r="E573" s="29" t="s">
@@ -20478,7 +20478,7 @@
         <v>619</v>
       </c>
       <c r="C574" s="20" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D574" s="29"/>
       <c r="E574" s="29" t="s">
@@ -20494,7 +20494,7 @@
         <v>17</v>
       </c>
       <c r="I574" s="20" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="575" spans="1:9" ht="30">
@@ -20505,7 +20505,7 @@
         <v>619</v>
       </c>
       <c r="C575" s="20" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D575" s="29"/>
       <c r="E575" s="29" t="s">
@@ -20530,7 +20530,7 @@
         <v>619</v>
       </c>
       <c r="C576" s="20" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="D576" s="29"/>
       <c r="E576" s="29" t="s">
@@ -20555,7 +20555,7 @@
         <v>619</v>
       </c>
       <c r="C577" s="20" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="D577" s="29"/>
       <c r="E577" s="29" t="s">
@@ -20580,7 +20580,7 @@
         <v>619</v>
       </c>
       <c r="C578" s="20" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="D578" s="29"/>
       <c r="E578" s="29" t="s">
@@ -20605,7 +20605,7 @@
         <v>619</v>
       </c>
       <c r="C579" s="20" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D579" s="29"/>
       <c r="E579" s="29" t="s">
@@ -20630,7 +20630,7 @@
         <v>619</v>
       </c>
       <c r="C580" s="20" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="D580" s="29"/>
       <c r="E580" s="29" t="s">
@@ -20646,7 +20646,7 @@
         <v>17</v>
       </c>
       <c r="I580" s="20" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="581" spans="1:10" ht="45">
@@ -20711,8 +20711,8 @@
       <c r="B583" s="30" t="s">
         <v>620</v>
       </c>
-      <c r="C583" s="32" t="s">
-        <v>1036</v>
+      <c r="C583" s="20" t="s">
+        <v>1374</v>
       </c>
       <c r="D583" s="29"/>
       <c r="E583" s="29" t="s">
@@ -20764,6 +20764,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -20771,96 +20776,91 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A583:B584 D583:I584 A20:I582">
-    <cfRule type="expression" dxfId="52" priority="79">
+    <cfRule type="expression" dxfId="52" priority="85">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="80">
+    <cfRule type="expression" dxfId="51" priority="86">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="87">
+    <cfRule type="expression" dxfId="50" priority="93">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A583:B584 D583:I584 A20:I582">
-    <cfRule type="expression" dxfId="49" priority="33">
+    <cfRule type="expression" dxfId="49" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="34">
+    <cfRule type="expression" dxfId="48" priority="40">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="35">
+    <cfRule type="expression" dxfId="47" priority="41">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F582:F584 G88 F20:F580">
-    <cfRule type="expression" dxfId="46" priority="39">
+    <cfRule type="expression" dxfId="46" priority="45">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="40">
+    <cfRule type="expression" dxfId="45" priority="46">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I582:I584">
-    <cfRule type="expression" dxfId="44" priority="30">
+    <cfRule type="expression" dxfId="44" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="31">
+    <cfRule type="expression" dxfId="43" priority="37">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="32">
+    <cfRule type="expression" dxfId="42" priority="38">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I582:I584">
-    <cfRule type="expression" dxfId="41" priority="27">
+    <cfRule type="expression" dxfId="41" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="28">
+    <cfRule type="expression" dxfId="40" priority="34">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="29">
+    <cfRule type="expression" dxfId="39" priority="35">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F581">
-    <cfRule type="expression" dxfId="38" priority="22">
+    <cfRule type="expression" dxfId="38" priority="28">
       <formula>NOT(VLOOKUP(F581,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="23">
+    <cfRule type="expression" dxfId="37" priority="29">
       <formula>(VLOOKUP(F581,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I581">
-    <cfRule type="expression" dxfId="36" priority="16">
+    <cfRule type="expression" dxfId="36" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="17">
+    <cfRule type="expression" dxfId="35" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="18">
+    <cfRule type="expression" dxfId="34" priority="24">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I581">
-    <cfRule type="expression" dxfId="33" priority="13">
+    <cfRule type="expression" dxfId="33" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="14">
+    <cfRule type="expression" dxfId="32" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="15">
+    <cfRule type="expression" dxfId="31" priority="21">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C583">
+  <conditionalFormatting sqref="C584">
     <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -20871,7 +20871,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C583">
+  <conditionalFormatting sqref="C584">
     <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -20882,7 +20882,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C584">
+  <conditionalFormatting sqref="C583">
     <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -20893,7 +20893,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C584">
+  <conditionalFormatting sqref="C583">
     <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>

</xml_diff>

<commit_message>
[MS-OXCNOTIF] fix watchman error issues
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="1375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4291" uniqueCount="1375">
   <si>
     <t>Req ID</t>
   </si>
@@ -4670,6 +4670,21 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4693,21 +4708,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5784,127 +5784,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5917,12 +5917,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -5935,12 +5935,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -5953,12 +5953,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -5971,60 +5971,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -10750,7 +10750,7 @@
         <v>15</v>
       </c>
       <c r="H201" s="29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I201" s="31"/>
     </row>
@@ -15236,7 +15236,9 @@
       <c r="H373" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I373" s="31"/>
+      <c r="I373" s="31" t="s">
+        <v>969</v>
+      </c>
     </row>
     <row r="374" spans="1:9" ht="45">
       <c r="A374" s="29" t="s">
@@ -16339,7 +16341,7 @@
         <v>7</v>
       </c>
       <c r="G417" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H417" s="29" t="s">
         <v>18</v>
@@ -16864,7 +16866,7 @@
         <v>7</v>
       </c>
       <c r="G438" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H438" s="29" t="s">
         <v>18</v>
@@ -20764,11 +20766,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -20776,6 +20773,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A583:B584 D583:I584 A20:I582">

</xml_diff>

<commit_message>
Updated version number for MS-OXCNOTIF RS file.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCNOTIF/MS-OXCNOTIF_RequirementSpecification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E0E583-E305-4D85-939F-D1D7A29B707A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249FFE90-F668-44EE-9B36-55BFFA4683C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4395,10 +4395,6 @@
     <t>[In Appendix A: Product Behavior] MessageFlags does specify the message flags of new mail that has been received.(Exchange 2007, Exchange 2010, Exchange 2016 and above follow this behavior.)</t>
   </si>
   <si>
-    <t>19.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">[In Appendix A: Product Behavior] &lt;6&gt; Section 2.2.1.3.3: Outlook 2013, Outlook 2016 andOutlook 2019 do not send the EcRRegisterPushNotification RPC method call. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4420,6 +4416,9 @@
   </si>
   <si>
     <t>[In RopRegisterNotification ROP Request Buffer] [NotificationTypes value] 0x0080: The server sends notifications to the client when SearchCompleted events occur within the scope of interest.</t>
+  </si>
+  <si>
+    <t>21.0</t>
   </si>
 </sst>
 </file>
@@ -4697,6 +4696,21 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4720,21 +4734,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5831,8 +5830,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K586"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5873,130 +5872,130 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>1371</v>
+        <v>1377</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="11">
-        <v>43374</v>
+        <v>44516</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
     </row>
     <row r="9" spans="1:9" ht="78.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="25" t="s">
@@ -6008,12 +6007,12 @@
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="26" t="s">
@@ -6025,12 +6024,12 @@
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="26" t="s">
@@ -6042,12 +6041,12 @@
       <c r="C14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="27" t="s">
@@ -6059,57 +6058,57 @@
       <c r="C15" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
     </row>
     <row r="17" spans="1:11" ht="64.5" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="46" t="s">
         <v>1366</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" ht="30">
@@ -6607,13 +6606,13 @@
     </row>
     <row r="38" spans="1:9" ht="30">
       <c r="A38" s="21" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>575</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D38" s="28"/>
       <c r="E38" s="28" t="s">
@@ -7427,7 +7426,7 @@
         <v>579</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="D70" s="28"/>
       <c r="E70" s="28" t="s">
@@ -18452,7 +18451,7 @@
         <v>617</v>
       </c>
       <c r="C497" s="19" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="D497" s="28"/>
       <c r="E497" s="28" t="s">
@@ -18477,7 +18476,7 @@
         <v>617</v>
       </c>
       <c r="C498" s="19" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D498" s="28" t="s">
         <v>908</v>
@@ -18504,7 +18503,7 @@
         <v>617</v>
       </c>
       <c r="C499" s="19" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D499" s="33" t="s">
         <v>1311</v>
@@ -20873,11 +20872,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -20885,6 +20879,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A584:B585 D584:I585 A509:I583 A162:B162 D162:I162 A163:I507 A20:I161">

</xml_diff>